<commit_message>
examples/cache: ran tests for ints and longs
</commit_message>
<xml_diff>
--- a/examples/cache/cache.xlsx
+++ b/examples/cache/cache.xlsx
@@ -7,7 +7,9 @@
     <workbookView xWindow="76940" yWindow="-500" windowWidth="30360" windowHeight="18240" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="cache" sheetId="1" r:id="rId1"/>
+    <sheet name="ints" sheetId="3" r:id="rId1"/>
+    <sheet name="longs" sheetId="2" r:id="rId2"/>
+    <sheet name="doubles" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
   <si>
     <t>stride</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -111,7 +113,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>cache!$B$1</c:f>
+              <c:f>ints!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -133,7 +135,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>cache!$A$2:$A$82</c:f>
+              <c:f>ints!$A$2:$A$82</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="81"/>
@@ -385,7 +387,1293 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>cache!$B$2:$B$82</c:f>
+              <c:f>ints!$B$2:$B$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="81"/>
+                <c:pt idx="0">
+                  <c:v>0.863805</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.578799</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.841355</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.09091</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.32528</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.57244</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.82146</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0643</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.31984</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.57195</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.91272</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.12194</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.672519999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.785</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.08088</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.18722</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.83007</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.56529</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.39683</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.69256</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.81505</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.96083</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7.01615</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7.08512</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7.26574</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.22297</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.278090000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8.57014</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8.82996</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9.22359</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8.87474</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>10.2029</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10.5533</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>11.1837</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9.7282</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8.49596</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8.22364</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>11.2512</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>12.4053</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>12.442</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>12.4499</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>12.439</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>12.4885</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>12.1883</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>12.4821</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>12.4688</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>8.638350000000001</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>9.53685</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>7.88895</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>7.88291</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>7.5392</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>6.29363</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>6.57021</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.90287</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.65823</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.14305</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.10553</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.25932</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.630381</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.09224</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.644401</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.38683</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.636976</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.640355</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.673493</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.670624</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.359983</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.350135</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.349522</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.376144</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.394436</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.387061</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.463857</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.456481</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.540378</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.600602</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.66071</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.720887</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.781183</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.841305</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.901233</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="560068632"/>
+        <c:axId val="560338856"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="560068632"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>stride</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="560338856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="560338856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="560068632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>time for strided copy of 1Gb worth of doubles</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>longs!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>charm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>longs!$A$2:$A$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="81"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>700.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>800.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>900.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7000.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9000.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>20000.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>30000.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40000.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>50000.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>60000.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>70000.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>80000.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>90000.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>200000.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>300000.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>400000.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>600000.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>700000.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>800000.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>900000.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.0E6</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.0E6</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.0E6</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.0E6</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>6.0E6</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>7.0E6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>8.0E6</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>9.0E6</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.0E7</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2.0E7</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.0E7</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4.0E7</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>5.0E7</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6.0E7</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>7.0E7</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>8.0E7</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>9.0E7</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.0E8</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2.0E8</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.0E8</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>4.0E8</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>5.0E8</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>6.0E8</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7.0E8</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>8.0E8</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>9.0E8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>longs!$B$2:$B$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="81"/>
+                <c:pt idx="0">
+                  <c:v>0.736978</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.18848</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.782421</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.03151</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.28636</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.55169</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.80256</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.06353</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.26112</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.45768</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.34617</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.54789</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.42381</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.20637</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.34246</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.32222</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.40688</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.43197</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.35161</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.50308</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.55487</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.65121</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.29711</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.71102</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.40428</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.79834</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.40441</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.4364</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.5321</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.40318</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.90346</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.15739</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7.17759</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.89258</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.51466</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.25263</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.63108</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6.2345</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6.23953</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6.10834</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>6.2521</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.66498</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5.51286</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5.5248</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.50978</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.36095</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.97071</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.7985</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3.33309</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.46288</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.954734</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.46274</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.04042</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.731883</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.743409</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.797852</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.713932</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.857443</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.51045</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.678751</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.52567</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.680914</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.523598</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.542775</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.278124</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.273367</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.29597</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.331396</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.271812</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.275059</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.289902</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.288268</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.283851</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.34338</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.397655</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.457745</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.517746</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.577933</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.638713</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.698344</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.759682</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="775965624"/>
+        <c:axId val="775980984"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="775965624"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>stride</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="775980984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="775980984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="775965624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>time for strided copy of 1Gb worth of doubles</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>doubles!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>charm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>doubles!$A$2:$A$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="81"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>700.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>800.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>900.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7000.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9000.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>20000.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>30000.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40000.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>50000.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>60000.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>70000.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>80000.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>90000.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>200000.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>300000.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>400000.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>600000.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>700000.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>800000.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>900000.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.0E6</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.0E6</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.0E6</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.0E6</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>6.0E6</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>7.0E6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>8.0E6</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>9.0E6</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.0E7</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2.0E7</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.0E7</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4.0E7</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>5.0E7</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6.0E7</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>7.0E7</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>8.0E7</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>9.0E7</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.0E8</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2.0E8</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.0E8</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>4.0E8</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>5.0E8</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>6.0E8</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7.0E8</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>8.0E8</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>9.0E8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>doubles!$B$2:$B$82</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="81"/>
@@ -642,7 +1930,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>cache!$C$1</c:f>
+              <c:f>doubles!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -681,7 +1969,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>cache!$A$2:$A$82</c:f>
+              <c:f>doubles!$A$2:$A$82</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="81"/>
@@ -933,7 +2221,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>cache!$C$2:$C$82</c:f>
+              <c:f>doubles!$C$2:$C$82</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="81"/>
@@ -1185,12 +2473,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="673385400"/>
-        <c:axId val="673382152"/>
+        <c:axId val="744987416"/>
+        <c:axId val="745134520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="673385400"/>
+        <c:axId val="744987416"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1220,12 +2507,12 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="673382152"/>
+        <c:crossAx val="745134520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="673382152"/>
+        <c:axId val="745134520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1251,7 +2538,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="673385400"/>
+        <c:crossAx val="744987416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1271,6 +2558,76 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1625,10 +2982,1369 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:B82"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B82"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.86380500000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.57879899999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.84135499999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1.09091</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1.32528</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1.5724400000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1.8214600000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2.0642999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>2.3198400000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>2.5719500000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>4.9127200000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>30</v>
+      </c>
+      <c r="B13">
+        <v>6.1219400000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>40</v>
+      </c>
+      <c r="B14">
+        <v>6.6725199999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <v>6.7850000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>60</v>
+      </c>
+      <c r="B16">
+        <v>7.0808799999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>70</v>
+      </c>
+      <c r="B17">
+        <v>7.1872199999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>80</v>
+      </c>
+      <c r="B18">
+        <v>6.8300700000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>90</v>
+      </c>
+      <c r="B19">
+        <v>6.5652900000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>100</v>
+      </c>
+      <c r="B20">
+        <v>6.3968299999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>200</v>
+      </c>
+      <c r="B21">
+        <v>6.6925600000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <v>300</v>
+      </c>
+      <c r="B22">
+        <v>6.8150500000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
+        <v>400</v>
+      </c>
+      <c r="B23">
+        <v>6.9608299999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>500</v>
+      </c>
+      <c r="B24">
+        <v>7.0161499999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25">
+        <v>600</v>
+      </c>
+      <c r="B25">
+        <v>7.0851199999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26">
+        <v>700</v>
+      </c>
+      <c r="B26">
+        <v>7.2657400000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27">
+        <v>800</v>
+      </c>
+      <c r="B27">
+        <v>7.2229700000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28">
+        <v>900</v>
+      </c>
+      <c r="B28">
+        <v>8.2780900000000006</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29">
+        <v>1000</v>
+      </c>
+      <c r="B29">
+        <v>8.5701400000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30">
+        <v>2000</v>
+      </c>
+      <c r="B30">
+        <v>8.8299599999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31">
+        <v>3000</v>
+      </c>
+      <c r="B31">
+        <v>9.2235899999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32">
+        <v>4000</v>
+      </c>
+      <c r="B32">
+        <v>8.8747399999999992</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33">
+        <v>5000</v>
+      </c>
+      <c r="B33">
+        <v>10.2029</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34">
+        <v>6000</v>
+      </c>
+      <c r="B34">
+        <v>10.5533</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35">
+        <v>7000</v>
+      </c>
+      <c r="B35">
+        <v>11.1837</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36">
+        <v>8000</v>
+      </c>
+      <c r="B36">
+        <v>9.7281999999999993</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37">
+        <v>9000</v>
+      </c>
+      <c r="B37">
+        <v>8.4959600000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38">
+        <v>10000</v>
+      </c>
+      <c r="B38">
+        <v>8.2236399999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39">
+        <v>20000</v>
+      </c>
+      <c r="B39">
+        <v>11.251200000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40">
+        <v>30000</v>
+      </c>
+      <c r="B40">
+        <v>12.4053</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41">
+        <v>40000</v>
+      </c>
+      <c r="B41">
+        <v>12.442</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42">
+        <v>50000</v>
+      </c>
+      <c r="B42">
+        <v>12.4499</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43">
+        <v>60000</v>
+      </c>
+      <c r="B43">
+        <v>12.439</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44">
+        <v>70000</v>
+      </c>
+      <c r="B44">
+        <v>12.4885</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45">
+        <v>80000</v>
+      </c>
+      <c r="B45">
+        <v>12.1883</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46">
+        <v>90000</v>
+      </c>
+      <c r="B46">
+        <v>12.482100000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47">
+        <v>100000</v>
+      </c>
+      <c r="B47">
+        <v>12.4688</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48">
+        <v>200000</v>
+      </c>
+      <c r="B48">
+        <v>8.6383500000000009</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49">
+        <v>300000</v>
+      </c>
+      <c r="B49">
+        <v>9.5368499999999994</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50">
+        <v>400000</v>
+      </c>
+      <c r="B50">
+        <v>7.8889500000000004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51">
+        <v>500000</v>
+      </c>
+      <c r="B51">
+        <v>7.8829099999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52">
+        <v>600000</v>
+      </c>
+      <c r="B52">
+        <v>7.5392000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53">
+        <v>700000</v>
+      </c>
+      <c r="B53">
+        <v>6.2936300000000003</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54">
+        <v>800000</v>
+      </c>
+      <c r="B54">
+        <v>6.5702100000000003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55">
+        <v>900000</v>
+      </c>
+      <c r="B55">
+        <v>1.9028700000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56">
+        <v>1000000</v>
+      </c>
+      <c r="B56">
+        <v>2.6582300000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57">
+        <v>2000000</v>
+      </c>
+      <c r="B57">
+        <v>1.1430499999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58">
+        <v>3000000</v>
+      </c>
+      <c r="B58">
+        <v>1.1055299999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59">
+        <v>4000000</v>
+      </c>
+      <c r="B59">
+        <v>1.25932</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60">
+        <v>5000000</v>
+      </c>
+      <c r="B60">
+        <v>0.63038099999999997</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61">
+        <v>6000000</v>
+      </c>
+      <c r="B61">
+        <v>1.0922400000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62">
+        <v>7000000</v>
+      </c>
+      <c r="B62">
+        <v>0.644401</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63">
+        <v>8000000</v>
+      </c>
+      <c r="B63">
+        <v>1.38683</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64">
+        <v>9000000</v>
+      </c>
+      <c r="B64">
+        <v>0.63697599999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65">
+        <v>10000000</v>
+      </c>
+      <c r="B65">
+        <v>0.64035500000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66">
+        <v>20000000</v>
+      </c>
+      <c r="B66">
+        <v>0.67349300000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67">
+        <v>30000000</v>
+      </c>
+      <c r="B67">
+        <v>0.670624</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68">
+        <v>40000000</v>
+      </c>
+      <c r="B68">
+        <v>0.359983</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69">
+        <v>50000000</v>
+      </c>
+      <c r="B69">
+        <v>0.35013499999999997</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70">
+        <v>60000000</v>
+      </c>
+      <c r="B70">
+        <v>0.349522</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71">
+        <v>70000000</v>
+      </c>
+      <c r="B71">
+        <v>0.37614399999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72">
+        <v>80000000</v>
+      </c>
+      <c r="B72">
+        <v>0.39443600000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73">
+        <v>90000000</v>
+      </c>
+      <c r="B73">
+        <v>0.38706099999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74">
+        <v>100000000</v>
+      </c>
+      <c r="B74">
+        <v>0.46385700000000002</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75">
+        <v>200000000</v>
+      </c>
+      <c r="B75">
+        <v>0.45648100000000003</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76">
+        <v>300000000</v>
+      </c>
+      <c r="B76">
+        <v>0.54037800000000002</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77">
+        <v>400000000</v>
+      </c>
+      <c r="B77">
+        <v>0.60060199999999997</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78">
+        <v>500000000</v>
+      </c>
+      <c r="B78">
+        <v>0.66071000000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79">
+        <v>600000000</v>
+      </c>
+      <c r="B79">
+        <v>0.72088700000000006</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80">
+        <v>700000000</v>
+      </c>
+      <c r="B80">
+        <v>0.78118299999999996</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81">
+        <v>800000000</v>
+      </c>
+      <c r="B81">
+        <v>0.84130499999999997</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82">
+        <v>900000000</v>
+      </c>
+      <c r="B82">
+        <v>0.90123299999999995</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:B82"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.73697800000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1.18848</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.78242100000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1.0315099999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1.2863599999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1.55169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1.8025599999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2.0635300000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>2.26112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>2.4576799999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>3.3461699999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>30</v>
+      </c>
+      <c r="B13">
+        <v>3.5478900000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>40</v>
+      </c>
+      <c r="B14">
+        <v>3.42381</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <v>3.2063700000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>60</v>
+      </c>
+      <c r="B16">
+        <v>3.34246</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>70</v>
+      </c>
+      <c r="B17">
+        <v>3.3222200000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>80</v>
+      </c>
+      <c r="B18">
+        <v>3.4068800000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>90</v>
+      </c>
+      <c r="B19">
+        <v>3.4319700000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>100</v>
+      </c>
+      <c r="B20">
+        <v>3.35161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>200</v>
+      </c>
+      <c r="B21">
+        <v>3.5030800000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <v>300</v>
+      </c>
+      <c r="B22">
+        <v>3.5548700000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
+        <v>400</v>
+      </c>
+      <c r="B23">
+        <v>3.6512099999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>500</v>
+      </c>
+      <c r="B24">
+        <v>4.29711</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25">
+        <v>600</v>
+      </c>
+      <c r="B25">
+        <v>4.7110200000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26">
+        <v>700</v>
+      </c>
+      <c r="B26">
+        <v>4.40428</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27">
+        <v>800</v>
+      </c>
+      <c r="B27">
+        <v>3.79834</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28">
+        <v>900</v>
+      </c>
+      <c r="B28">
+        <v>4.4044100000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29">
+        <v>1000</v>
+      </c>
+      <c r="B29">
+        <v>4.4363999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30">
+        <v>2000</v>
+      </c>
+      <c r="B30">
+        <v>4.5320999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31">
+        <v>3000</v>
+      </c>
+      <c r="B31">
+        <v>5.4031799999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32">
+        <v>4000</v>
+      </c>
+      <c r="B32">
+        <v>4.9034599999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33">
+        <v>5000</v>
+      </c>
+      <c r="B33">
+        <v>4.1573900000000004</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34">
+        <v>6000</v>
+      </c>
+      <c r="B34">
+        <v>7.1775900000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35">
+        <v>7000</v>
+      </c>
+      <c r="B35">
+        <v>4.8925799999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36">
+        <v>8000</v>
+      </c>
+      <c r="B36">
+        <v>6.5146600000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37">
+        <v>9000</v>
+      </c>
+      <c r="B37">
+        <v>5.2526299999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38">
+        <v>10000</v>
+      </c>
+      <c r="B38">
+        <v>5.6310799999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39">
+        <v>20000</v>
+      </c>
+      <c r="B39">
+        <v>6.2344999999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40">
+        <v>30000</v>
+      </c>
+      <c r="B40">
+        <v>6.2395300000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41">
+        <v>40000</v>
+      </c>
+      <c r="B41">
+        <v>6.1083400000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42">
+        <v>50000</v>
+      </c>
+      <c r="B42">
+        <v>6.2521000000000004</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43">
+        <v>60000</v>
+      </c>
+      <c r="B43">
+        <v>5.6649799999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44">
+        <v>70000</v>
+      </c>
+      <c r="B44">
+        <v>5.5128599999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45">
+        <v>80000</v>
+      </c>
+      <c r="B45">
+        <v>5.5247999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46">
+        <v>90000</v>
+      </c>
+      <c r="B46">
+        <v>4.5097800000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47">
+        <v>100000</v>
+      </c>
+      <c r="B47">
+        <v>4.3609499999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48">
+        <v>200000</v>
+      </c>
+      <c r="B48">
+        <v>3.97071</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49">
+        <v>300000</v>
+      </c>
+      <c r="B49">
+        <v>3.7985000000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50">
+        <v>400000</v>
+      </c>
+      <c r="B50">
+        <v>3.3330899999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51">
+        <v>500000</v>
+      </c>
+      <c r="B51">
+        <v>1.46288</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52">
+        <v>600000</v>
+      </c>
+      <c r="B52">
+        <v>0.95473399999999997</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53">
+        <v>700000</v>
+      </c>
+      <c r="B53">
+        <v>2.4627400000000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54">
+        <v>800000</v>
+      </c>
+      <c r="B54">
+        <v>1.0404199999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55">
+        <v>900000</v>
+      </c>
+      <c r="B55">
+        <v>0.73188299999999995</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56">
+        <v>1000000</v>
+      </c>
+      <c r="B56">
+        <v>0.74340899999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57">
+        <v>2000000</v>
+      </c>
+      <c r="B57">
+        <v>0.79785200000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58">
+        <v>3000000</v>
+      </c>
+      <c r="B58">
+        <v>0.71393200000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59">
+        <v>4000000</v>
+      </c>
+      <c r="B59">
+        <v>0.85744299999999996</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60">
+        <v>5000000</v>
+      </c>
+      <c r="B60">
+        <v>0.51044999999999996</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61">
+        <v>6000000</v>
+      </c>
+      <c r="B61">
+        <v>0.67875099999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62">
+        <v>7000000</v>
+      </c>
+      <c r="B62">
+        <v>0.52566999999999997</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63">
+        <v>8000000</v>
+      </c>
+      <c r="B63">
+        <v>0.68091400000000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64">
+        <v>9000000</v>
+      </c>
+      <c r="B64">
+        <v>0.52359800000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65">
+        <v>10000000</v>
+      </c>
+      <c r="B65">
+        <v>0.54277500000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66">
+        <v>20000000</v>
+      </c>
+      <c r="B66">
+        <v>0.27812399999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67">
+        <v>30000000</v>
+      </c>
+      <c r="B67">
+        <v>0.27336700000000003</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68">
+        <v>40000000</v>
+      </c>
+      <c r="B68">
+        <v>0.29597000000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69">
+        <v>50000000</v>
+      </c>
+      <c r="B69">
+        <v>0.33139600000000002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70">
+        <v>60000000</v>
+      </c>
+      <c r="B70">
+        <v>0.271812</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71">
+        <v>70000000</v>
+      </c>
+      <c r="B71">
+        <v>0.275059</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72">
+        <v>80000000</v>
+      </c>
+      <c r="B72">
+        <v>0.28990199999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73">
+        <v>90000000</v>
+      </c>
+      <c r="B73">
+        <v>0.28826800000000002</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74">
+        <v>100000000</v>
+      </c>
+      <c r="B74">
+        <v>0.28385100000000002</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75">
+        <v>200000000</v>
+      </c>
+      <c r="B75">
+        <v>0.34338000000000002</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76">
+        <v>300000000</v>
+      </c>
+      <c r="B76">
+        <v>0.39765499999999998</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77">
+        <v>400000000</v>
+      </c>
+      <c r="B77">
+        <v>0.45774500000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78">
+        <v>500000000</v>
+      </c>
+      <c r="B78">
+        <v>0.51774600000000004</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79">
+        <v>600000000</v>
+      </c>
+      <c r="B79">
+        <v>0.57793300000000003</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80">
+        <v>700000000</v>
+      </c>
+      <c r="B80">
+        <v>0.63871299999999998</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81">
+        <v>800000000</v>
+      </c>
+      <c r="B81">
+        <v>0.69834399999999996</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82">
+        <v>900000000</v>
+      </c>
+      <c r="B82">
+        <v>0.75968199999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C82"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -2536,6 +5252,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>